<commit_message>
ADD 'CLOSEBROWSER' to UIOperation
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="KeywordFramework" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Keyword</t>
   </si>
@@ -55,12 +55,6 @@
     <t>TestCase</t>
   </si>
   <si>
-    <t>Reset Login In Application</t>
-  </si>
-  <si>
-    <t>Login In Application</t>
-  </si>
-  <si>
     <t>resetButton</t>
   </si>
   <si>
@@ -68,13 +62,25 @@
   </si>
   <si>
     <t>mgr!23</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Login In Application</t>
+  </si>
+  <si>
+    <t>CLOSEBROWSER</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Navigate to the WebApp</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Reset Login In Application</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +88,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,7 +123,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,10 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,165 +472,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add TC verification(assertEquals); Add TCs(Err Hand + Positive); Refactoring
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="o7032SJrUYCbjSJahVa3tHyKW+30Fnh6DC85aAcYgdh8Oohh1wj3TS/m/K+54l9Pqh4/DIa1jFrTT5wQGsAjgQ==" workbookSaltValue="Cvg/1FRpudUyBYKAzd/OfQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="5520" tabRatio="331"/>
   </bookViews>
   <sheets>
-    <sheet name="KeywordFramework" sheetId="1" r:id="rId1"/>
+    <sheet name="UItests" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Keyword</t>
   </si>
@@ -25,9 +26,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>SETTEXT</t>
   </si>
   <si>
@@ -61,9 +59,6 @@
     <t>mgr123</t>
   </si>
   <si>
-    <t>mgr!23</t>
-  </si>
-  <si>
     <t>TC # 01.02 - Login In Application</t>
   </si>
   <si>
@@ -74,13 +69,55 @@
   </si>
   <si>
     <t>TC # 01.03 - Reset Login In Application</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Guru99 Bank Home Page</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Check Lenta</t>
+  </si>
+  <si>
+    <t>lenta</t>
+  </si>
+  <si>
+    <t>Enter your email id</t>
+  </si>
+  <si>
+    <t>mgr!2</t>
+  </si>
+  <si>
+    <t>VERIFYTITLE</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/V4/</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/V</t>
+  </si>
+  <si>
+    <t>mngr111078</t>
+  </si>
+  <si>
+    <t>EdevetY</t>
+  </si>
+  <si>
+    <t>Guru99 Bank Manager HomePage</t>
+  </si>
+  <si>
+    <t>logoutButton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,8 +150,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +181,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,18 +221,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,33 +545,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -506,42 +579,50 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
+      <c r="E3" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -549,150 +630,244 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
+      <c r="B10" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1"/>
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E17" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UIOperation.class - add CLOSEALERT operation. add Handling 404 to VERIFYTITLE operation
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -83,9 +83,6 @@
     <t>TC # 01.04 - Check Lenta</t>
   </si>
   <si>
-    <t>lenta</t>
-  </si>
-  <si>
     <t>Enter your email id</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>http://demo.guru99.com/V4/</t>
   </si>
   <si>
-    <t>http://demo.guru99.com/V</t>
-  </si>
-  <si>
     <t>mngr111078</t>
   </si>
   <si>
@@ -111,6 +105,12 @@
   </si>
   <si>
     <t>logoutButton</t>
+  </si>
+  <si>
+    <t>CLOSEALERT</t>
+  </si>
+  <si>
+    <t>You Have Succesfully Logged Out!!</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -237,9 +237,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -545,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +595,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -607,7 +608,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -626,7 +627,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -645,7 +646,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -653,14 +654,14 @@
       <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -675,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -689,12 +690,12 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
@@ -703,7 +704,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -712,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -721,10 +722,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -751,8 +756,8 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="13" t="s">
-        <v>27</v>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,8 +786,8 @@
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>24</v>
+      <c r="E19" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -796,7 +801,6 @@
       <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -824,13 +828,13 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>19</v>
@@ -839,35 +843,23 @@
         <v>18</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>